<commit_message>
Fix numeric column data type
</commit_message>
<xml_diff>
--- a/podatki/podatki_1.xlsx
+++ b/podatki/podatki_1.xlsx
@@ -451,10 +451,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="B2" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -463,10 +461,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="B3" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="4">
@@ -475,10 +471,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="B4" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="5">
@@ -487,10 +481,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="B5" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +491,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="B6" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -511,10 +501,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="B7" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="8">
@@ -523,10 +511,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="B8" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -535,10 +521,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="B9" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -547,10 +531,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="B10" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="11">
@@ -559,10 +541,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="B11" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="12">
@@ -571,10 +551,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="B12" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -583,10 +561,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+      <c r="B13" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -595,10 +571,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="B14" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -607,10 +581,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="B15" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -619,10 +591,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="B16" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="17">
@@ -631,10 +601,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="B17" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +611,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="B18" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -655,10 +621,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="B19" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="20">
@@ -667,10 +631,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="B20" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="21">
@@ -679,10 +641,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="B21" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="22">
@@ -691,10 +651,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
+      <c r="B22" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="23">
@@ -703,10 +661,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="B23" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="24">
@@ -715,10 +671,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="B24" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="25">
@@ -727,10 +681,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
+      <c r="B25" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="26">
@@ -739,10 +691,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="B26" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="27">
@@ -751,10 +701,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="B27" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="28">
@@ -763,10 +711,8 @@
           <t>da</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="B28" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="29">
@@ -775,10 +721,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="B29" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="30">
@@ -787,10 +731,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>67</t>
-        </is>
+      <c r="B30" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="31">
@@ -799,10 +741,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="B31" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="32">
@@ -811,10 +751,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="B32" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="33">
@@ -823,10 +761,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="B33" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="34">
@@ -835,10 +771,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="B34" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="35">
@@ -847,10 +781,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="B35" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="36">
@@ -859,10 +791,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
+      <c r="B36" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="37">
@@ -871,10 +801,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="B37" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="38">
@@ -883,10 +811,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="B38" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="39">
@@ -895,10 +821,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="B39" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="40">
@@ -907,10 +831,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="B40" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="41">
@@ -919,10 +841,8 @@
           <t>ne</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="B41" t="n">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>